<commit_message>
added Zeiss Apochromat 40x
</commit_message>
<xml_diff>
--- a/scale_bar_distances.xlsx
+++ b/scale_bar_distances.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristian/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristian/Desktop/moose-ch/scale_bar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64435A80-CE3B-074F-9B81-0FFA3F2B935B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A344111E-2A98-FA4A-87E4-63D87CF5679E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="1300" windowWidth="28040" windowHeight="17440" xr2:uid="{79376080-564F-C04B-A064-C243679E778C}"/>
+    <workbookView xWindow="1040" yWindow="460" windowWidth="24560" windowHeight="15540" xr2:uid="{79376080-564F-C04B-A064-C243679E778C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="81">
   <si>
     <t>Camera</t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>913</t>
+  </si>
+  <si>
+    <t>Apochromat 40x</t>
+  </si>
+  <si>
+    <t>873</t>
   </si>
 </sst>
 </file>
@@ -365,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -378,6 +384,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B459EB7-FADE-ED41-AEF2-429BC716563C}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -857,59 +864,62 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="10">
-        <v>6240</v>
-      </c>
-      <c r="F6" s="10">
-        <v>4160</v>
-      </c>
-      <c r="G6" s="10" t="s">
+      <c r="E6" s="6">
+        <v>6240</v>
+      </c>
+      <c r="F6" s="6">
+        <v>4160</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="4">
         <v>50</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="6">
-        <v>6240</v>
-      </c>
-      <c r="F7" s="6">
-        <v>4160</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>24</v>
+      <c r="I6" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="10">
+        <v>6240</v>
+      </c>
+      <c r="F7" s="10">
+        <v>4160</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="9">
+        <v>50</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -920,7 +930,7 @@
         <v>56</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="6">
         <v>6240</v>
@@ -929,10 +939,10 @@
         <v>4160</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>24</v>
@@ -946,7 +956,7 @@
         <v>56</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" s="6">
         <v>6240</v>
@@ -955,7 +965,7 @@
         <v>4160</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>28</v>
@@ -972,7 +982,7 @@
         <v>56</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" s="6">
         <v>6240</v>
@@ -981,13 +991,13 @@
         <v>4160</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -998,7 +1008,7 @@
         <v>56</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" s="6">
         <v>6240</v>
@@ -1007,7 +1017,7 @@
         <v>4160</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>15</v>
@@ -1024,7 +1034,7 @@
         <v>56</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="6">
         <v>6240</v>
@@ -1033,7 +1043,7 @@
         <v>4160</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>15</v>
@@ -1050,7 +1060,7 @@
         <v>56</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" s="6">
         <v>6240</v>
@@ -1059,7 +1069,7 @@
         <v>4160</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>15</v>
@@ -1076,7 +1086,7 @@
         <v>56</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E14" s="6">
         <v>6240</v>
@@ -1085,10 +1095,10 @@
         <v>4160</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>6</v>
@@ -1102,7 +1112,7 @@
         <v>56</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E15" s="6">
         <v>6240</v>
@@ -1111,7 +1121,7 @@
         <v>4160</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>17</v>
@@ -1120,57 +1130,57 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="10" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="6">
+        <v>6240</v>
+      </c>
+      <c r="F16" s="6">
+        <v>4160</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="10">
-        <v>6240</v>
-      </c>
-      <c r="F16" s="10">
-        <v>4160</v>
-      </c>
-      <c r="G16" s="10" t="s">
+      <c r="E17" s="10">
+        <v>6240</v>
+      </c>
+      <c r="F17" s="10">
+        <v>4160</v>
+      </c>
+      <c r="G17" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H17" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="6">
-        <v>6240</v>
-      </c>
-      <c r="F17" s="6">
-        <v>4160</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>24</v>
+      <c r="I17" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1181,7 +1191,7 @@
         <v>44</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" s="6">
         <v>6240</v>
@@ -1190,10 +1200,10 @@
         <v>4160</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>24</v>
@@ -1207,7 +1217,7 @@
         <v>44</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" s="6">
         <v>6240</v>
@@ -1216,7 +1226,7 @@
         <v>4160</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>28</v>
@@ -1233,75 +1243,75 @@
         <v>44</v>
       </c>
       <c r="D20" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="6">
+        <v>6240</v>
+      </c>
+      <c r="F20" s="6">
+        <v>4160</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="6">
-        <v>6240</v>
-      </c>
-      <c r="F20" s="6">
-        <v>4160</v>
-      </c>
-      <c r="G20" s="6" t="s">
+      <c r="E21" s="6">
+        <v>6240</v>
+      </c>
+      <c r="F21" s="6">
+        <v>4160</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10" t="s">
+      <c r="I21" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D22" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="10">
-        <v>6240</v>
-      </c>
-      <c r="F21" s="10">
-        <v>4160</v>
-      </c>
-      <c r="G21" s="10" t="s">
+      <c r="E22" s="10">
+        <v>6240</v>
+      </c>
+      <c r="F22" s="10">
+        <v>4160</v>
+      </c>
+      <c r="G22" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="H22" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I21" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="6">
-        <v>6240</v>
-      </c>
-      <c r="F22" s="6">
-        <v>4160</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>24</v>
+      <c r="I22" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1312,7 +1322,7 @@
         <v>43</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E23" s="6">
         <v>6240</v>
@@ -1321,7 +1331,7 @@
         <v>4160</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>28</v>
@@ -1338,7 +1348,7 @@
         <v>43</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" s="6">
         <v>6240</v>
@@ -1347,10 +1357,10 @@
         <v>4160</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>24</v>
@@ -1364,7 +1374,7 @@
         <v>43</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" s="6">
         <v>6240</v>
@@ -1373,7 +1383,7 @@
         <v>4160</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>31</v>
@@ -1386,52 +1396,78 @@
       <c r="A26" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D26" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="6">
+        <v>6240</v>
+      </c>
+      <c r="F26" s="6">
+        <v>4160</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="6">
-        <v>6240</v>
-      </c>
-      <c r="F26" s="6">
-        <v>4160</v>
-      </c>
-      <c r="G26" s="6" t="s">
+      <c r="E27" s="6">
+        <v>6240</v>
+      </c>
+      <c r="F27" s="6">
+        <v>4160</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="11" t="s">
+      <c r="I27" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D28" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="10">
-        <v>6240</v>
-      </c>
-      <c r="F27" s="10">
-        <v>4160</v>
-      </c>
-      <c r="G27" s="10" t="s">
+      <c r="E28" s="10">
+        <v>6240</v>
+      </c>
+      <c r="F28" s="10">
+        <v>4160</v>
+      </c>
+      <c r="G28" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="H28" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I27" s="7" t="s">
+      <c r="I28" s="7" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added Canon EOS R6 MArk II
</commit_message>
<xml_diff>
--- a/scale_bar_distances.xlsx
+++ b/scale_bar_distances.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristian/Desktop/liverworts/scale_bar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453B20C9-3ED1-2947-8630-5BCFAEDC8BFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6C8473-6AAA-DD4F-B209-C50DEC34535F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="460" windowWidth="24560" windowHeight="15540" xr2:uid="{79376080-564F-C04B-A064-C243679E778C}"/>
+    <workbookView xWindow="1040" yWindow="500" windowWidth="26400" windowHeight="20040" xr2:uid="{79376080-564F-C04B-A064-C243679E778C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="147">
   <si>
     <t>Camera</t>
   </si>
@@ -304,6 +304,168 @@
   </si>
   <si>
     <t>599</t>
+  </si>
+  <si>
+    <t>Canon EOS R6 Mark II</t>
+  </si>
+  <si>
+    <t>Neofluar 100x</t>
+  </si>
+  <si>
+    <t>100x</t>
+  </si>
+  <si>
+    <t>6000</t>
+  </si>
+  <si>
+    <t>4000</t>
+  </si>
+  <si>
+    <t>1.5x</t>
+  </si>
+  <si>
+    <t>1.0x</t>
+  </si>
+  <si>
+    <t>2.0x</t>
+  </si>
+  <si>
+    <t>251</t>
+  </si>
+  <si>
+    <t>335</t>
+  </si>
+  <si>
+    <t>425</t>
+  </si>
+  <si>
+    <t>505</t>
+  </si>
+  <si>
+    <t>584</t>
+  </si>
+  <si>
+    <t>671</t>
+  </si>
+  <si>
+    <t>751</t>
+  </si>
+  <si>
+    <t>840</t>
+  </si>
+  <si>
+    <t>172</t>
+  </si>
+  <si>
+    <t>432</t>
+  </si>
+  <si>
+    <t>487</t>
+  </si>
+  <si>
+    <t>570</t>
+  </si>
+  <si>
+    <t>658</t>
+  </si>
+  <si>
+    <t>740</t>
+  </si>
+  <si>
+    <t>804</t>
+  </si>
+  <si>
+    <t>1159</t>
+  </si>
+  <si>
+    <t>1227</t>
+  </si>
+  <si>
+    <t>1296</t>
+  </si>
+  <si>
+    <t>1363</t>
+  </si>
+  <si>
+    <t>1433</t>
+  </si>
+  <si>
+    <t>1499</t>
+  </si>
+  <si>
+    <t>1565</t>
+  </si>
+  <si>
+    <t>1665</t>
+  </si>
+  <si>
+    <t>267</t>
+  </si>
+  <si>
+    <t>328</t>
+  </si>
+  <si>
+    <t>415</t>
+  </si>
+  <si>
+    <t>524</t>
+  </si>
+  <si>
+    <t>662</t>
+  </si>
+  <si>
+    <t>834</t>
+  </si>
+  <si>
+    <t>1058</t>
+  </si>
+  <si>
+    <t>1372</t>
+  </si>
+  <si>
+    <t>1726</t>
+  </si>
+  <si>
+    <t>2152</t>
+  </si>
+  <si>
+    <t>1075</t>
+  </si>
+  <si>
+    <t>208</t>
+  </si>
+  <si>
+    <t>418</t>
+  </si>
+  <si>
+    <t>1675</t>
+  </si>
+  <si>
+    <t>4148</t>
+  </si>
+  <si>
+    <t>Laowa 85mm f/5.6</t>
+  </si>
+  <si>
+    <t>0.5x</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>198</t>
+  </si>
+  <si>
+    <t>278</t>
+  </si>
+  <si>
+    <t>325</t>
+  </si>
+  <si>
+    <t>MP-E</t>
+  </si>
+  <si>
+    <t>Laowa</t>
   </si>
 </sst>
 </file>
@@ -439,7 +601,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -727,7 +889,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -735,22 +897,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B459EB7-FADE-ED41-AEF2-429BC716563C}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="19" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.1640625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" style="4" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="6" customWidth="1"/>
     <col min="9" max="9" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -777,7 +939,7 @@
       <c r="G1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -806,7 +968,7 @@
       <c r="G2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -835,7 +997,7 @@
       <c r="G3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -864,7 +1026,7 @@
       <c r="G4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="6" t="s">
         <v>19</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -893,7 +1055,7 @@
       <c r="G5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="6" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -922,7 +1084,7 @@
       <c r="G6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="6">
         <v>50</v>
       </c>
       <c r="I6" s="12" t="s">
@@ -951,7 +1113,7 @@
       <c r="G7" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="10">
         <v>50</v>
       </c>
       <c r="I7" s="7" t="s">
@@ -980,7 +1142,7 @@
       <c r="G8" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="6" t="s">
         <v>69</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -1009,7 +1171,7 @@
       <c r="G9" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="6" t="s">
         <v>28</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -1038,7 +1200,7 @@
       <c r="G10" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="6" t="s">
         <v>28</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -1067,7 +1229,7 @@
       <c r="G11" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -1096,7 +1258,7 @@
       <c r="G12" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -1125,7 +1287,7 @@
       <c r="G13" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -1154,7 +1316,7 @@
       <c r="G14" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -1183,7 +1345,7 @@
       <c r="G15" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -1212,7 +1374,7 @@
       <c r="G16" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -1241,7 +1403,7 @@
       <c r="G17" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="H17" s="9" t="s">
+      <c r="H17" s="10" t="s">
         <v>17</v>
       </c>
       <c r="I17" s="7" t="s">
@@ -1252,6 +1414,9 @@
       <c r="A18" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="B18" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="C18" s="6" t="s">
         <v>44</v>
       </c>
@@ -1267,7 +1432,7 @@
       <c r="G18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="6" t="s">
         <v>26</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -1278,6 +1443,9 @@
       <c r="A19" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="B19" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="C19" s="6" t="s">
         <v>44</v>
       </c>
@@ -1293,7 +1461,7 @@
       <c r="G19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="6" t="s">
         <v>28</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -1304,6 +1472,9 @@
       <c r="A20" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="B20" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="C20" s="6" t="s">
         <v>44</v>
       </c>
@@ -1319,7 +1490,7 @@
       <c r="G20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="6" t="s">
         <v>28</v>
       </c>
       <c r="I20" s="1" t="s">
@@ -1330,6 +1501,9 @@
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="B21" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="C21" s="6" t="s">
         <v>44</v>
       </c>
@@ -1345,7 +1519,7 @@
       <c r="G21" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H21" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I21" s="1" t="s">
@@ -1356,7 +1530,9 @@
       <c r="A22" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="10"/>
+      <c r="B22" s="10" t="s">
+        <v>145</v>
+      </c>
       <c r="C22" s="10" t="s">
         <v>44</v>
       </c>
@@ -1372,7 +1548,7 @@
       <c r="G22" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H22" s="9" t="s">
+      <c r="H22" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I22" s="7" t="s">
@@ -1383,6 +1559,9 @@
       <c r="A23" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="B23" s="6" t="s">
+        <v>146</v>
+      </c>
       <c r="C23" s="6" t="s">
         <v>43</v>
       </c>
@@ -1398,7 +1577,7 @@
       <c r="G23" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="6" t="s">
         <v>28</v>
       </c>
       <c r="I23" s="1" t="s">
@@ -1409,6 +1588,9 @@
       <c r="A24" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="B24" s="6" t="s">
+        <v>146</v>
+      </c>
       <c r="C24" s="6" t="s">
         <v>43</v>
       </c>
@@ -1424,7 +1606,7 @@
       <c r="G24" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H24" s="6" t="s">
         <v>28</v>
       </c>
       <c r="I24" s="1" t="s">
@@ -1435,6 +1617,9 @@
       <c r="A25" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="B25" s="6" t="s">
+        <v>146</v>
+      </c>
       <c r="C25" s="6" t="s">
         <v>43</v>
       </c>
@@ -1450,7 +1635,7 @@
       <c r="G25" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H25" s="6" t="s">
         <v>31</v>
       </c>
       <c r="I25" s="1" t="s">
@@ -1461,6 +1646,9 @@
       <c r="A26" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="B26" s="6" t="s">
+        <v>146</v>
+      </c>
       <c r="C26" s="6" t="s">
         <v>43</v>
       </c>
@@ -1476,7 +1664,7 @@
       <c r="G26" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H26" s="6" t="s">
         <v>31</v>
       </c>
       <c r="I26" s="1" t="s">
@@ -1487,6 +1675,9 @@
       <c r="A27" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="B27" s="6" t="s">
+        <v>146</v>
+      </c>
       <c r="C27" s="8" t="s">
         <v>43</v>
       </c>
@@ -1502,7 +1693,7 @@
       <c r="G27" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H27" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -1513,7 +1704,9 @@
       <c r="A28" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="10"/>
+      <c r="B28" s="10" t="s">
+        <v>146</v>
+      </c>
       <c r="C28" s="11" t="s">
         <v>43</v>
       </c>
@@ -1529,7 +1722,7 @@
       <c r="G28" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="H28" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I28" s="7" t="s">
@@ -1558,7 +1751,7 @@
       <c r="G29" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I29" s="1" t="s">
@@ -1587,7 +1780,7 @@
       <c r="G30" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="H30" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I30" s="1" t="s">
@@ -1616,7 +1809,7 @@
       <c r="G31" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="H31" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I31" s="1" t="s">
@@ -1645,7 +1838,7 @@
       <c r="G32" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="H32" s="4" t="s">
+      <c r="H32" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I32" s="1" t="s">
@@ -1674,7 +1867,7 @@
       <c r="G33" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="H33" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I33" s="1" t="s">
@@ -1703,7 +1896,7 @@
       <c r="G34" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="H34" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I34" s="1" t="s">
@@ -1732,7 +1925,7 @@
       <c r="G35" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="H35" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I35" s="1" t="s">
@@ -1761,11 +1954,1258 @@
       <c r="G36" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="H36" s="9" t="s">
+      <c r="H36" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="I36" s="7" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="H52" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I57" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H61" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I61" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="H62" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I62" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I63" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I64" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G65" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="H65" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I65" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H68" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H70" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F71" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G71" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="H71" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I71" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H74" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="H76" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H78" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F79" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G79" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="H79" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I79" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update of distances for R6 M II
</commit_message>
<xml_diff>
--- a/scale_bar_distances.xlsx
+++ b/scale_bar_distances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristian/Desktop/liverworts/scale_bar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6C8473-6AAA-DD4F-B209-C50DEC34535F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ADF7BC-CE14-C949-815A-88C1E2E99D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="500" windowWidth="26400" windowHeight="20040" xr2:uid="{79376080-564F-C04B-A064-C243679E778C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="148">
   <si>
     <t>Camera</t>
   </si>
@@ -330,21 +330,6 @@
     <t>2.0x</t>
   </si>
   <si>
-    <t>251</t>
-  </si>
-  <si>
-    <t>335</t>
-  </si>
-  <si>
-    <t>425</t>
-  </si>
-  <si>
-    <t>505</t>
-  </si>
-  <si>
-    <t>584</t>
-  </si>
-  <si>
     <t>671</t>
   </si>
   <si>
@@ -354,18 +339,6 @@
     <t>840</t>
   </si>
   <si>
-    <t>172</t>
-  </si>
-  <si>
-    <t>432</t>
-  </si>
-  <si>
-    <t>487</t>
-  </si>
-  <si>
-    <t>570</t>
-  </si>
-  <si>
     <t>658</t>
   </si>
   <si>
@@ -387,30 +360,6 @@
     <t>1363</t>
   </si>
   <si>
-    <t>1433</t>
-  </si>
-  <si>
-    <t>1499</t>
-  </si>
-  <si>
-    <t>1565</t>
-  </si>
-  <si>
-    <t>1665</t>
-  </si>
-  <si>
-    <t>267</t>
-  </si>
-  <si>
-    <t>328</t>
-  </si>
-  <si>
-    <t>415</t>
-  </si>
-  <si>
-    <t>524</t>
-  </si>
-  <si>
     <t>662</t>
   </si>
   <si>
@@ -420,52 +369,106 @@
     <t>1058</t>
   </si>
   <si>
-    <t>1372</t>
-  </si>
-  <si>
-    <t>1726</t>
-  </si>
-  <si>
-    <t>2152</t>
-  </si>
-  <si>
     <t>1075</t>
   </si>
   <si>
-    <t>208</t>
-  </si>
-  <si>
-    <t>418</t>
-  </si>
-  <si>
-    <t>1675</t>
-  </si>
-  <si>
-    <t>4148</t>
-  </si>
-  <si>
     <t>Laowa 85mm f/5.6</t>
   </si>
   <si>
     <t>0.5x</t>
   </si>
   <si>
-    <t>83</t>
-  </si>
-  <si>
-    <t>198</t>
-  </si>
-  <si>
-    <t>278</t>
-  </si>
-  <si>
-    <t>325</t>
-  </si>
-  <si>
     <t>MP-E</t>
   </si>
   <si>
     <t>Laowa</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>838</t>
+  </si>
+  <si>
+    <t>830</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>836</t>
+  </si>
+  <si>
+    <t>1040</t>
+  </si>
+  <si>
+    <t>686</t>
+  </si>
+  <si>
+    <t>863</t>
+  </si>
+  <si>
+    <t>1076</t>
+  </si>
+  <si>
+    <t>1024</t>
+  </si>
+  <si>
+    <t>656</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1068</t>
+  </si>
+  <si>
+    <t>1168</t>
+  </si>
+  <si>
+    <t>1010</t>
+  </si>
+  <si>
+    <t>850</t>
+  </si>
+  <si>
+    <t>1005</t>
+  </si>
+  <si>
+    <t>753</t>
+  </si>
+  <si>
+    <t>975</t>
+  </si>
+  <si>
+    <t>1112</t>
+  </si>
+  <si>
+    <t>792</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>864</t>
+  </si>
+  <si>
+    <t>974</t>
+  </si>
+  <si>
+    <t>1140</t>
+  </si>
+  <si>
+    <t>717</t>
+  </si>
+  <si>
+    <t>750</t>
+  </si>
+  <si>
+    <t>782</t>
+  </si>
+  <si>
+    <t>833</t>
   </si>
 </sst>
 </file>
@@ -899,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B459EB7-FADE-ED41-AEF2-429BC716563C}">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1415,7 +1418,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>44</v>
@@ -1444,7 +1447,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>44</v>
@@ -1473,7 +1476,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>44</v>
@@ -1502,7 +1505,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>44</v>
@@ -1531,7 +1534,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>44</v>
@@ -1560,7 +1563,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>43</v>
@@ -1589,7 +1592,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>43</v>
@@ -1618,7 +1621,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>43</v>
@@ -1647,7 +1650,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>43</v>
@@ -1676,7 +1679,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>43</v>
@@ -1705,7 +1708,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>43</v>
@@ -1981,13 +1984,13 @@
         <v>97</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -2010,10 +2013,10 @@
         <v>97</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>6</v>
@@ -2039,10 +2042,10 @@
         <v>97</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>6</v>
@@ -2068,7 +2071,7 @@
         <v>97</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>21</v>
@@ -2097,10 +2100,10 @@
         <v>97</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>21</v>
+        <v>119</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>6</v>
@@ -2126,10 +2129,10 @@
         <v>97</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>6</v>
@@ -2155,10 +2158,10 @@
         <v>97</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>24</v>
@@ -2184,10 +2187,10 @@
         <v>97</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>24</v>
@@ -2213,10 +2216,10 @@
         <v>97</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>24</v>
@@ -2242,10 +2245,10 @@
         <v>97</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>24</v>
@@ -2271,7 +2274,7 @@
         <v>97</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>31</v>
@@ -2300,7 +2303,7 @@
         <v>97</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="H48" s="6" t="s">
         <v>31</v>
@@ -2329,7 +2332,7 @@
         <v>97</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="H49" s="6" t="s">
         <v>31</v>
@@ -2358,13 +2361,13 @@
         <v>97</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
@@ -2387,13 +2390,13 @@
         <v>97</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2416,13 +2419,13 @@
         <v>97</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H52" s="10" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -2430,7 +2433,7 @@
         <v>93</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>44</v>
@@ -2445,10 +2448,10 @@
         <v>97</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>109</v>
+        <v>20</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>24</v>
@@ -2459,7 +2462,7 @@
         <v>93</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>44</v>
@@ -2474,10 +2477,10 @@
         <v>97</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>101</v>
+        <v>136</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>24</v>
@@ -2488,7 +2491,7 @@
         <v>93</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>44</v>
@@ -2503,10 +2506,10 @@
         <v>97</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>24</v>
@@ -2517,7 +2520,7 @@
         <v>93</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>44</v>
@@ -2532,10 +2535,10 @@
         <v>97</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>24</v>
@@ -2546,7 +2549,7 @@
         <v>93</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>44</v>
@@ -2561,10 +2564,10 @@
         <v>97</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I57" s="12" t="s">
         <v>24</v>
@@ -2575,7 +2578,7 @@
         <v>93</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>44</v>
@@ -2590,10 +2593,10 @@
         <v>97</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>24</v>
@@ -2604,7 +2607,7 @@
         <v>93</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>44</v>
@@ -2619,7 +2622,7 @@
         <v>97</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>31</v>
@@ -2633,7 +2636,7 @@
         <v>93</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>44</v>
@@ -2648,7 +2651,7 @@
         <v>97</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H60" s="6" t="s">
         <v>31</v>
@@ -2662,7 +2665,7 @@
         <v>93</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>44</v>
@@ -2677,7 +2680,7 @@
         <v>97</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H61" s="10" t="s">
         <v>31</v>
@@ -2691,25 +2694,25 @@
         <v>93</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="D62" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H62" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="H62" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="I62" s="12" t="s">
         <v>24</v>
@@ -2720,10 +2723,10 @@
         <v>93</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>99</v>
@@ -2735,10 +2738,10 @@
         <v>97</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="I63" s="12" t="s">
         <v>24</v>
@@ -2749,10 +2752,10 @@
         <v>93</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>98</v>
@@ -2764,10 +2767,10 @@
         <v>97</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="I64" s="12" t="s">
         <v>24</v>
@@ -2778,10 +2781,10 @@
         <v>93</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="D65" s="10" t="s">
         <v>100</v>
@@ -2793,10 +2796,10 @@
         <v>97</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="H65" s="10" t="s">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="I65" s="7" t="s">
         <v>24</v>
@@ -2807,7 +2810,7 @@
         <v>93</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>43</v>
@@ -2822,10 +2825,10 @@
         <v>97</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>24</v>
@@ -2836,7 +2839,7 @@
         <v>93</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>43</v>
@@ -2851,10 +2854,10 @@
         <v>97</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I67" s="1" t="s">
         <v>24</v>
@@ -2865,7 +2868,7 @@
         <v>93</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>43</v>
@@ -2880,10 +2883,10 @@
         <v>97</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>24</v>
@@ -2894,7 +2897,7 @@
         <v>93</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>43</v>
@@ -2909,7 +2912,7 @@
         <v>97</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="H69" s="6" t="s">
         <v>31</v>
@@ -2923,7 +2926,7 @@
         <v>93</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>43</v>
@@ -2938,7 +2941,7 @@
         <v>97</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="H70" s="6" t="s">
         <v>31</v>
@@ -2952,7 +2955,7 @@
         <v>93</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>43</v>
@@ -2967,7 +2970,7 @@
         <v>97</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="H71" s="10" t="s">
         <v>31</v>
@@ -2996,13 +2999,13 @@
         <v>97</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
@@ -3025,13 +3028,13 @@
         <v>97</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
@@ -3054,13 +3057,13 @@
         <v>97</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -3083,13 +3086,13 @@
         <v>97</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -3112,13 +3115,13 @@
         <v>97</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -3141,13 +3144,13 @@
         <v>97</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
@@ -3170,13 +3173,13 @@
         <v>97</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -3199,13 +3202,13 @@
         <v>97</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="H79" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I79" s="7" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added macro distances for Canon EOS R5
</commit_message>
<xml_diff>
--- a/scale_bar_distances.xlsx
+++ b/scale_bar_distances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristian/Desktop/liverworts/scale_bar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ADF7BC-CE14-C949-815A-88C1E2E99D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8706F38B-09C8-6041-89F9-27A389379544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="500" windowWidth="26400" windowHeight="20040" xr2:uid="{79376080-564F-C04B-A064-C243679E778C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="168">
   <si>
     <t>Camera</t>
   </si>
@@ -469,6 +469,66 @@
   </si>
   <si>
     <t>833</t>
+  </si>
+  <si>
+    <t>Canon EOS R5</t>
+  </si>
+  <si>
+    <t>8192</t>
+  </si>
+  <si>
+    <t>5464</t>
+  </si>
+  <si>
+    <t>0.75x</t>
+  </si>
+  <si>
+    <t>Mitutoyo</t>
+  </si>
+  <si>
+    <t>Mitutoyo 7.5x</t>
+  </si>
+  <si>
+    <t>7.5x</t>
+  </si>
+  <si>
+    <t>Mitutoyo HR 5.0x</t>
+  </si>
+  <si>
+    <t>1188</t>
+  </si>
+  <si>
+    <t>674</t>
+  </si>
+  <si>
+    <t>783</t>
+  </si>
+  <si>
+    <t>898</t>
+  </si>
+  <si>
+    <t>1012</t>
+  </si>
+  <si>
+    <t>925</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>798</t>
+  </si>
+  <si>
+    <t>633</t>
+  </si>
+  <si>
+    <t>889</t>
+  </si>
+  <si>
+    <t>1218</t>
+  </si>
+  <si>
+    <t>919</t>
   </si>
 </sst>
 </file>
@@ -572,7 +632,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -585,7 +645,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -900,10 +959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B459EB7-FADE-ED41-AEF2-429BC716563C}">
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="G80" sqref="G80"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="I93" sqref="I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1065,7 +1124,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -1090,7 +1149,7 @@
       <c r="H6" s="6">
         <v>50</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2544,7 +2603,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>93</v>
       </c>
@@ -2569,7 +2628,7 @@
       <c r="H57" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I57" s="12" t="s">
+      <c r="I57" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2689,7 +2748,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>93</v>
       </c>
@@ -2714,11 +2773,11 @@
       <c r="H62" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="I62" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I62" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>93</v>
       </c>
@@ -2743,11 +2802,11 @@
       <c r="H63" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="I63" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I63" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>93</v>
       </c>
@@ -2772,7 +2831,7 @@
       <c r="H64" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="I64" s="12" t="s">
+      <c r="I64" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3207,7 +3266,384 @@
       <c r="H79" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I79" s="1" t="s">
+      <c r="I79" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="H81" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="H82" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H83" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G84" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="H84" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D85" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F85" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G85" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H85" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I85" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G87" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="H87" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F88" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H88" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G89" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="H89" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C90" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D90" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F90" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G90" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="H90" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I90" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E91" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F91" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G91" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="H91" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D92" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F92" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G92" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="H92" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I92" s="7" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated scales for Mitutoyo on R6 M II
</commit_message>
<xml_diff>
--- a/scale_bar_distances.xlsx
+++ b/scale_bar_distances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristian/Desktop/liverworts/scale_bar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8706F38B-09C8-6041-89F9-27A389379544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E8271D-B216-B64C-9965-A5DABB118FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="500" windowWidth="26400" windowHeight="20040" xr2:uid="{79376080-564F-C04B-A064-C243679E778C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="170">
   <si>
     <t>Camera</t>
   </si>
@@ -529,6 +529,12 @@
   </si>
   <si>
     <t>919</t>
+  </si>
+  <si>
+    <t>892</t>
+  </si>
+  <si>
+    <t>673</t>
   </si>
 </sst>
 </file>
@@ -959,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B459EB7-FADE-ED41-AEF2-429BC716563C}">
-  <dimension ref="A1:I92"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="I93" sqref="I93"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="G95" sqref="G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3647,6 +3653,64 @@
         <v>6</v>
       </c>
     </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G93" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="H93" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B94" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C94" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D94" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F94" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G94" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="H94" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I94" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added 40x and 63x Oil objectives
</commit_message>
<xml_diff>
--- a/scale_bar_distances.xlsx
+++ b/scale_bar_distances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristian/Desktop/liverworts/scale_bar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E7FEB7-BB76-7748-95C5-020748CEF6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB46B5D-8CC3-D542-AFC1-974727981C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="500" windowWidth="26400" windowHeight="20040" xr2:uid="{79376080-564F-C04B-A064-C243679E778C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="203">
   <si>
     <t>Camera</t>
   </si>
@@ -598,6 +598,42 @@
   </si>
   <si>
     <t>1143</t>
+  </si>
+  <si>
+    <t>Apochromat 40x Oil</t>
+  </si>
+  <si>
+    <t>Neofluar 40x Oil</t>
+  </si>
+  <si>
+    <t>Neofluar 63x Oil</t>
+  </si>
+  <si>
+    <t>Apochromat 63x Oil</t>
+  </si>
+  <si>
+    <t>63x</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>1120</t>
+  </si>
+  <si>
+    <t>1136</t>
+  </si>
+  <si>
+    <t>884</t>
+  </si>
+  <si>
+    <t>822</t>
+  </si>
+  <si>
+    <t>832</t>
+  </si>
+  <si>
+    <t>649</t>
   </si>
 </sst>
 </file>
@@ -721,7 +757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -734,7 +770,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
@@ -1051,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B459EB7-FADE-ED41-AEF2-429BC716563C}">
-  <dimension ref="A1:I108"/>
+  <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2115,7 +2150,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>93</v>
       </c>
@@ -2140,7 +2175,7 @@
       <c r="H37" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I37" s="12" t="s">
+      <c r="I37" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2289,7 +2324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>93</v>
       </c>
@@ -2297,10 +2332,10 @@
         <v>8</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>95</v>
+        <v>38</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>96</v>
@@ -2309,41 +2344,41 @@
         <v>97</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>147</v>
+        <v>200</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="I43" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B44" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="G44" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="H44" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="I44" s="14" t="s">
+      <c r="C44" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="I44" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2352,13 +2387,13 @@
         <v>93</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>56</v>
+        <v>193</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>96</v>
@@ -2367,13 +2402,13 @@
         <v>97</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>131</v>
+        <v>202</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>69</v>
+        <v>196</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -2381,13 +2416,13 @@
         <v>93</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>56</v>
+        <v>194</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>58</v>
+        <v>195</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>96</v>
@@ -2399,10 +2434,10 @@
         <v>129</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>28</v>
+        <v>196</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -2410,13 +2445,13 @@
         <v>93</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>56</v>
+        <v>179</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>96</v>
@@ -2425,42 +2460,42 @@
         <v>97</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>24</v>
+        <v>122</v>
+      </c>
+      <c r="I47" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="H48" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -2474,7 +2509,7 @@
         <v>56</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>96</v>
@@ -2483,10 +2518,10 @@
         <v>97</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>24</v>
@@ -2503,7 +2538,7 @@
         <v>56</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>96</v>
@@ -2512,10 +2547,10 @@
         <v>97</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>24</v>
@@ -2532,7 +2567,7 @@
         <v>56</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>96</v>
@@ -2541,10 +2576,10 @@
         <v>97</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>24</v>
@@ -2561,7 +2596,7 @@
         <v>56</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>96</v>
@@ -2570,13 +2605,13 @@
         <v>97</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -2590,7 +2625,7 @@
         <v>56</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>96</v>
@@ -2599,42 +2634,42 @@
         <v>97</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B54" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D54" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="G54" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="H54" s="10" t="s">
-        <v>17</v>
+      <c r="D54" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
@@ -2642,13 +2677,13 @@
         <v>93</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>117</v>
+        <v>56</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>96</v>
@@ -2657,10 +2692,10 @@
         <v>97</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>20</v>
+        <v>113</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>24</v>
@@ -2671,13 +2706,13 @@
         <v>93</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>117</v>
+        <v>56</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>96</v>
@@ -2686,13 +2721,13 @@
         <v>97</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>130</v>
+        <v>17</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
@@ -2700,13 +2735,13 @@
         <v>93</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>117</v>
+        <v>56</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>96</v>
@@ -2715,42 +2750,42 @@
         <v>97</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>130</v>
+        <v>17</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="H58" s="6" t="s">
-        <v>28</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="H58" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -2764,7 +2799,7 @@
         <v>44</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>96</v>
@@ -2773,10 +2808,10 @@
         <v>97</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>133</v>
+        <v>20</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>24</v>
@@ -2793,7 +2828,7 @@
         <v>44</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>96</v>
@@ -2802,10 +2837,10 @@
         <v>97</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>24</v>
@@ -2822,7 +2857,7 @@
         <v>44</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>96</v>
@@ -2831,10 +2866,10 @@
         <v>97</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>24</v>
@@ -2851,7 +2886,7 @@
         <v>44</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>96</v>
@@ -2860,41 +2895,41 @@
         <v>97</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B63" s="10" t="s">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B63" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C63" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D63" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="G63" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="H63" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I63" s="7" t="s">
+      <c r="D63" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I63" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2903,13 +2938,13 @@
         <v>93</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>115</v>
+        <v>44</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>116</v>
+        <v>46</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>96</v>
@@ -2918,10 +2953,10 @@
         <v>97</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>140</v>
+        <v>28</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>24</v>
@@ -2932,13 +2967,13 @@
         <v>93</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>115</v>
+        <v>44</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>99</v>
+        <v>47</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>96</v>
@@ -2947,10 +2982,10 @@
         <v>97</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>139</v>
+        <v>101</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>24</v>
@@ -2961,13 +2996,13 @@
         <v>93</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>115</v>
+        <v>44</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>96</v>
@@ -2976,10 +3011,10 @@
         <v>97</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>24</v>
@@ -2990,13 +3025,13 @@
         <v>93</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>115</v>
+        <v>44</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="E67" s="10" t="s">
         <v>96</v>
@@ -3005,10 +3040,10 @@
         <v>97</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="H67" s="10" t="s">
-        <v>130</v>
+        <v>31</v>
       </c>
       <c r="I67" s="7" t="s">
         <v>24</v>
@@ -3022,10 +3057,10 @@
         <v>118</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>43</v>
+        <v>115</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>34</v>
+        <v>116</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>96</v>
@@ -3034,10 +3069,10 @@
         <v>97</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>28</v>
+        <v>140</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>24</v>
@@ -3051,10 +3086,10 @@
         <v>118</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>43</v>
+        <v>115</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>96</v>
@@ -3063,10 +3098,10 @@
         <v>97</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>24</v>
@@ -3080,10 +3115,10 @@
         <v>118</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>43</v>
+        <v>115</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>96</v>
@@ -3092,41 +3127,41 @@
         <v>97</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B71" s="6" t="s">
+    <row r="71" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B71" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C71" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="G71" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="H71" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I71" s="1" t="s">
+      <c r="C71" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F71" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G71" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H71" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="I71" s="7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3137,11 +3172,11 @@
       <c r="B72" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C72" s="8" t="s">
+      <c r="C72" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>96</v>
@@ -3150,41 +3185,41 @@
         <v>97</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B73" s="10" t="s">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B73" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="C73" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D73" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E73" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F73" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="G73" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="H73" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I73" s="7" t="s">
+      <c r="D73" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I73" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3193,13 +3228,13 @@
         <v>93</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>96</v>
@@ -3208,13 +3243,13 @@
         <v>97</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -3222,13 +3257,13 @@
         <v>93</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>96</v>
@@ -3237,13 +3272,13 @@
         <v>97</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -3251,13 +3286,13 @@
         <v>93</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C76" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C76" s="8" t="s">
         <v>43</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>96</v>
@@ -3266,42 +3301,42 @@
         <v>97</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C77" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C77" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D77" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="G77" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H77" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I77" s="1" t="s">
-        <v>6</v>
+      <c r="D77" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F77" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G77" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H77" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I77" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
@@ -3315,7 +3350,7 @@
         <v>43</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>96</v>
@@ -3324,10 +3359,10 @@
         <v>97</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>144</v>
+        <v>107</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I78" s="1" t="s">
         <v>6</v>
@@ -3344,7 +3379,7 @@
         <v>43</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="E79" s="6" t="s">
         <v>96</v>
@@ -3353,10 +3388,10 @@
         <v>97</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>6</v>
@@ -3373,7 +3408,7 @@
         <v>43</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>96</v>
@@ -3382,41 +3417,41 @@
         <v>97</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B81" s="10" t="s">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B81" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C81" s="10" t="s">
+      <c r="C81" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D81" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="E81" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F81" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="G81" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="H81" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I81" s="7" t="s">
+      <c r="D81" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H81" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I81" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3425,13 +3460,13 @@
         <v>93</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>152</v>
+        <v>81</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>155</v>
+        <v>43</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>96</v>
@@ -3440,27 +3475,27 @@
         <v>97</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="H82" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I82" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>93</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>152</v>
+        <v>81</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>153</v>
+        <v>43</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>154</v>
+        <v>82</v>
       </c>
       <c r="E83" s="6" t="s">
         <v>96</v>
@@ -3469,12 +3504,12 @@
         <v>97</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="H83" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I83" s="12" t="s">
+      <c r="I83" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3483,13 +3518,13 @@
         <v>93</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>152</v>
+        <v>81</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>170</v>
+        <v>43</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>172</v>
+        <v>83</v>
       </c>
       <c r="E84" s="6" t="s">
         <v>96</v>
@@ -3498,10 +3533,10 @@
         <v>97</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
       <c r="H84" s="6" t="s">
-        <v>175</v>
+        <v>17</v>
       </c>
       <c r="I84" s="1" t="s">
         <v>6</v>
@@ -3512,80 +3547,80 @@
         <v>93</v>
       </c>
       <c r="B85" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D85" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F85" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G85" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="H85" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I85" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B86" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C85" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="D85" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="E85" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F85" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="G85" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="H85" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I85" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="C86" s="6" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>149</v>
+        <v>96</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>150</v>
+        <v>97</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="H86" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I86" s="12" t="s">
+      <c r="I86" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>148</v>
+        <v>93</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>8</v>
+        <v>152</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>11</v>
+        <v>153</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>34</v>
+        <v>154</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>149</v>
+        <v>96</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>150</v>
+        <v>97</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="H87" s="6" t="s">
         <v>17</v>
@@ -3596,59 +3631,59 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
-        <v>148</v>
+        <v>93</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>8</v>
+        <v>152</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>13</v>
+        <v>170</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>35</v>
+        <v>172</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>149</v>
+        <v>96</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>150</v>
+        <v>97</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>17</v>
+        <v>175</v>
       </c>
       <c r="I88" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A89" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F89" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="G89" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="H89" s="6" t="s">
+    <row r="89" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C89" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="D89" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E89" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F89" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G89" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="H89" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I89" s="1" t="s">
+      <c r="I89" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3660,10 +3695,10 @@
         <v>8</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>10</v>
+        <v>180</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>149</v>
@@ -3672,10 +3707,10 @@
         <v>150</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="H90" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I90" s="1" t="s">
         <v>6</v>
@@ -3689,10 +3724,10 @@
         <v>8</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>79</v>
+        <v>11</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E91" s="6" t="s">
         <v>149</v>
@@ -3701,16 +3736,16 @@
         <v>150</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="H91" s="6" t="s">
-        <v>119</v>
+        <v>17</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>148</v>
       </c>
@@ -3718,10 +3753,10 @@
         <v>8</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>179</v>
+        <v>13</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="E92" s="6" t="s">
         <v>149</v>
@@ -3730,41 +3765,41 @@
         <v>150</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="H92" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="I92" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B93" s="10" t="s">
+      <c r="B93" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C93" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D93" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E93" s="10" t="s">
+      <c r="C93" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E93" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F93" s="10" t="s">
+      <c r="F93" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="G93" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="H93" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="I93" s="14" t="s">
+      <c r="G93" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="H93" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I93" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3773,13 +3808,13 @@
         <v>148</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>118</v>
+        <v>8</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E94" s="6" t="s">
         <v>149</v>
@@ -3788,13 +3823,13 @@
         <v>150</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>156</v>
+        <v>187</v>
       </c>
       <c r="H94" s="6" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
@@ -3802,13 +3837,13 @@
         <v>148</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>118</v>
+        <v>8</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E95" s="6" t="s">
         <v>149</v>
@@ -3817,10 +3852,10 @@
         <v>150</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>157</v>
+        <v>188</v>
       </c>
       <c r="H95" s="6" t="s">
-        <v>15</v>
+        <v>119</v>
       </c>
       <c r="I95" s="1" t="s">
         <v>6</v>
@@ -3831,13 +3866,13 @@
         <v>148</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>118</v>
+        <v>8</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>43</v>
+        <v>192</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E96" s="6" t="s">
         <v>149</v>
@@ -3846,10 +3881,10 @@
         <v>150</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="H96" s="6" t="s">
-        <v>15</v>
+        <v>119</v>
       </c>
       <c r="I96" s="1" t="s">
         <v>6</v>
@@ -3860,13 +3895,13 @@
         <v>148</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>118</v>
+        <v>8</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>43</v>
+        <v>191</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E97" s="6" t="s">
         <v>149</v>
@@ -3875,10 +3910,10 @@
         <v>150</v>
       </c>
       <c r="G97" s="6" t="s">
-        <v>159</v>
+        <v>198</v>
       </c>
       <c r="H97" s="6" t="s">
-        <v>15</v>
+        <v>119</v>
       </c>
       <c r="I97" s="1" t="s">
         <v>6</v>
@@ -3889,13 +3924,13 @@
         <v>148</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C98" s="8" t="s">
-        <v>43</v>
+        <v>8</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>193</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>48</v>
+        <v>195</v>
       </c>
       <c r="E98" s="6" t="s">
         <v>149</v>
@@ -3904,41 +3939,41 @@
         <v>150</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>160</v>
+        <v>199</v>
       </c>
       <c r="H98" s="6" t="s">
-        <v>15</v>
+        <v>196</v>
       </c>
       <c r="I98" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="9" t="s">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B99" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="C99" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D99" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E99" s="10" t="s">
+      <c r="B99" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="E99" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F99" s="10" t="s">
+      <c r="F99" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="G99" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H99" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I99" s="7" t="s">
+      <c r="G99" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="H99" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="I99" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3947,13 +3982,13 @@
         <v>148</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>118</v>
+        <v>8</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>115</v>
+        <v>179</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="E100" s="6" t="s">
         <v>149</v>
@@ -3962,42 +3997,42 @@
         <v>150</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>161</v>
+        <v>189</v>
       </c>
       <c r="H100" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="I100" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A101" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="I100" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B101" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D101" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E101" s="6" t="s">
+      <c r="B101" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C101" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D101" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E101" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="F101" s="6" t="s">
+      <c r="F101" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="G101" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="H101" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I101" s="1" t="s">
-        <v>24</v>
+      <c r="G101" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="H101" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="I101" s="13" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
@@ -4008,10 +4043,10 @@
         <v>118</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>115</v>
+        <v>43</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>99</v>
+        <v>34</v>
       </c>
       <c r="E102" s="6" t="s">
         <v>149</v>
@@ -4020,10 +4055,10 @@
         <v>150</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>90</v>
+        <v>156</v>
       </c>
       <c r="H102" s="6" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="I102" s="1" t="s">
         <v>24</v>
@@ -4037,10 +4072,10 @@
         <v>118</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>115</v>
+        <v>43</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="E103" s="6" t="s">
         <v>149</v>
@@ -4049,42 +4084,42 @@
         <v>150</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="H103" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B104" s="10" t="s">
+      <c r="B104" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C104" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="D104" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="E104" s="10" t="s">
+      <c r="C104" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E104" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F104" s="10" t="s">
+      <c r="F104" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="G104" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="H104" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I104" s="7" t="s">
-        <v>24</v>
+      <c r="G104" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="H104" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
@@ -4092,13 +4127,13 @@
         <v>148</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>155</v>
+        <v>43</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E105" s="6" t="s">
         <v>149</v>
@@ -4107,7 +4142,7 @@
         <v>150</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="H105" s="6" t="s">
         <v>15</v>
@@ -4116,18 +4151,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>148</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C106" s="6" t="s">
-        <v>153</v>
+        <v>118</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>154</v>
+        <v>48</v>
       </c>
       <c r="E106" s="6" t="s">
         <v>149</v>
@@ -4136,70 +4171,302 @@
         <v>150</v>
       </c>
       <c r="G106" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="H106" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I106" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C107" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D107" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E107" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F107" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G107" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H107" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I107" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A108" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F108" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G108" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="H108" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A109" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E109" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F109" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G109" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="H109" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A110" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E110" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F110" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G110" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H110" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E111" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F111" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G111" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="H111" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B112" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C112" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D112" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E112" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F112" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G112" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="H112" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I112" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A113" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E113" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F113" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G113" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="H113" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E114" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F114" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G114" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="H106" s="6" t="s">
+      <c r="H114" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I106" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="4" t="s">
+      <c r="I114" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B107" s="6" t="s">
+      <c r="B115" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C107" s="6" t="s">
+      <c r="C115" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="D107" s="6" t="s">
+      <c r="D115" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="E107" s="6" t="s">
+      <c r="E115" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F107" s="6" t="s">
+      <c r="F115" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="G107" s="6" t="s">
+      <c r="G115" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H107" s="6" t="s">
+      <c r="H115" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="I107" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="9" t="s">
+      <c r="I115" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B108" s="10" t="s">
+      <c r="B116" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="C108" s="10" t="s">
+      <c r="C116" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="D108" s="10" t="s">
+      <c r="D116" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="E108" s="10" t="s">
+      <c r="E116" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="F108" s="10" t="s">
+      <c r="F116" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="G108" s="10" t="s">
+      <c r="G116" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="H108" s="10" t="s">
+      <c r="H116" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I108" s="14" t="s">
+      <c r="I116" s="13" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added Neofluar and Apochromat Oil objectives
</commit_message>
<xml_diff>
--- a/scale_bar_distances.xlsx
+++ b/scale_bar_distances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristian/Desktop/liverworts/scale_bar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB46B5D-8CC3-D542-AFC1-974727981C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD572FA-1958-2141-A18F-1F0C1B0AE34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="500" windowWidth="26400" windowHeight="20040" xr2:uid="{79376080-564F-C04B-A064-C243679E778C}"/>
+    <workbookView xWindow="7920" yWindow="500" windowWidth="26400" windowHeight="20040" xr2:uid="{79376080-564F-C04B-A064-C243679E778C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -600,9 +600,6 @@
     <t>1143</t>
   </si>
   <si>
-    <t>Apochromat 40x Oil</t>
-  </si>
-  <si>
     <t>Neofluar 40x Oil</t>
   </si>
   <si>
@@ -634,6 +631,9 @@
   </si>
   <si>
     <t>649</t>
+  </si>
+  <si>
+    <t>Oilapochromat 40x Oil</t>
   </si>
 </sst>
 </file>
@@ -1088,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B459EB7-FADE-ED41-AEF2-429BC716563C}">
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2332,7 +2332,7 @@
         <v>8</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>38</v>
@@ -2344,7 +2344,7 @@
         <v>97</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H43" s="6" t="s">
         <v>119</v>
@@ -2361,7 +2361,7 @@
         <v>8</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>38</v>
@@ -2373,7 +2373,7 @@
         <v>97</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H44" s="6" t="s">
         <v>119</v>
@@ -2390,22 +2390,22 @@
         <v>8</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D45" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H45" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="H45" s="6" t="s">
-        <v>196</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>6</v>
@@ -2419,10 +2419,10 @@
         <v>8</v>
       </c>
       <c r="C46" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D46" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>195</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>96</v>
@@ -2434,7 +2434,7 @@
         <v>129</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>6</v>
@@ -3869,7 +3869,7 @@
         <v>8</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D96" s="6" t="s">
         <v>38</v>
@@ -3881,7 +3881,7 @@
         <v>150</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H96" s="6" t="s">
         <v>119</v>
@@ -3898,7 +3898,7 @@
         <v>8</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="D97" s="6" t="s">
         <v>38</v>
@@ -3910,7 +3910,7 @@
         <v>150</v>
       </c>
       <c r="G97" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H97" s="6" t="s">
         <v>119</v>
@@ -3927,10 +3927,10 @@
         <v>8</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E98" s="6" t="s">
         <v>149</v>
@@ -3939,10 +3939,10 @@
         <v>150</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H98" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I98" s="1" t="s">
         <v>6</v>
@@ -3956,10 +3956,10 @@
         <v>8</v>
       </c>
       <c r="C99" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D99" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="D99" s="6" t="s">
-        <v>195</v>
       </c>
       <c r="E99" s="6" t="s">
         <v>149</v>
@@ -3971,7 +3971,7 @@
         <v>168</v>
       </c>
       <c r="H99" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>6</v>

</xml_diff>